<commit_message>
Nice formatted date for graph axis
</commit_message>
<xml_diff>
--- a/src/main/resources/MedicationLog.xlsx
+++ b/src/main/resources/MedicationLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catha\Documents\Health\ADHD\Evaluations\MedicationLog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57737EF0-A769-4AD1-A5DE-10D6C46D57C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB2414A-3300-494B-B6FA-39EF2F0FC732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="50" windowWidth="34980" windowHeight="21600" xr2:uid="{9F186BFD-4414-4B76-A6F8-859374025043}"/>
+    <workbookView xWindow="-38510" yWindow="-60" windowWidth="35200" windowHeight="21820" xr2:uid="{9F186BFD-4414-4B76-A6F8-859374025043}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>2nd Peak BP Time</t>
+  </si>
+  <si>
+    <t>Strong neck/ear pulse</t>
+  </si>
+  <si>
+    <t>Medication</t>
+  </si>
+  <si>
+    <t>Methylphenidate</t>
   </si>
 </sst>
 </file>
@@ -466,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB2C611-5CB2-4DA3-8535-A036389AD9E4}">
-  <dimension ref="A1:T32"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,10 +501,11 @@
     <col min="17" max="17" width="13.7265625" customWidth="1"/>
     <col min="18" max="18" width="14.26953125" customWidth="1"/>
     <col min="19" max="19" width="16.54296875" customWidth="1"/>
-    <col min="20" max="20" width="10.54296875" customWidth="1"/>
+    <col min="20" max="20" width="29.453125" customWidth="1"/>
+    <col min="21" max="21" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,8 +566,11 @@
       <c r="T1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45582</v>
       </c>
@@ -574,8 +587,11 @@
         <v>58</v>
       </c>
       <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45583</v>
       </c>
@@ -604,6 +620,9 @@
         <v>7</v>
       </c>
       <c r="J3" s="2"/>
+      <c r="N3">
+        <v>10</v>
+      </c>
       <c r="O3" s="2">
         <v>0.58194444444444449</v>
       </c>
@@ -611,8 +630,11 @@
       <c r="T3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45584</v>
       </c>
@@ -641,6 +663,9 @@
         <v>8</v>
       </c>
       <c r="J4" s="2"/>
+      <c r="N4">
+        <v>10</v>
+      </c>
       <c r="O4" s="2">
         <v>0.5805555555555556</v>
       </c>
@@ -648,8 +673,11 @@
       <c r="T4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45585</v>
       </c>
@@ -675,6 +703,9 @@
         <v>9</v>
       </c>
       <c r="J5" s="2"/>
+      <c r="N5">
+        <v>10</v>
+      </c>
       <c r="O5" s="2">
         <v>0.6020833333333333</v>
       </c>
@@ -682,8 +713,11 @@
       <c r="T5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45586</v>
       </c>
@@ -709,6 +743,9 @@
         <v>9</v>
       </c>
       <c r="J6" s="2"/>
+      <c r="N6">
+        <v>10</v>
+      </c>
       <c r="O6" s="2">
         <v>0.60416666666666663</v>
       </c>
@@ -716,8 +753,11 @@
       <c r="T6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45587</v>
       </c>
@@ -743,6 +783,9 @@
         <v>9</v>
       </c>
       <c r="J7" s="2"/>
+      <c r="N7">
+        <v>10</v>
+      </c>
       <c r="O7" s="2">
         <v>0.61597222222222225</v>
       </c>
@@ -750,8 +793,11 @@
       <c r="T7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45588</v>
       </c>
@@ -777,6 +823,9 @@
         <v>11</v>
       </c>
       <c r="J8" s="2"/>
+      <c r="N8">
+        <v>10</v>
+      </c>
       <c r="O8" s="2">
         <v>0.61111111111111116</v>
       </c>
@@ -784,8 +833,11 @@
       <c r="T8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45589</v>
       </c>
@@ -808,12 +860,18 @@
         <v>0.4236111111111111</v>
       </c>
       <c r="J9" s="2"/>
+      <c r="N9">
+        <v>10</v>
+      </c>
       <c r="O9" s="2">
         <v>0.59375</v>
       </c>
       <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>45590</v>
       </c>
@@ -839,12 +897,18 @@
         <v>13</v>
       </c>
       <c r="J10" s="2"/>
+      <c r="N10">
+        <v>20</v>
+      </c>
       <c r="O10" s="2">
         <v>0.59722222222222221</v>
       </c>
       <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>45591</v>
       </c>
@@ -870,12 +934,18 @@
         <v>13</v>
       </c>
       <c r="J11" s="2"/>
+      <c r="N11">
+        <v>20</v>
+      </c>
       <c r="O11" s="2">
         <v>0.64583333333333337</v>
       </c>
       <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>45592</v>
       </c>
@@ -901,12 +971,18 @@
         <v>14</v>
       </c>
       <c r="J12" s="2"/>
+      <c r="N12">
+        <v>20</v>
+      </c>
       <c r="O12" s="2">
         <v>0.58333333333333337</v>
       </c>
       <c r="P12" s="2"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>45593</v>
       </c>
@@ -932,12 +1008,18 @@
         <v>0.38055555555555554</v>
       </c>
       <c r="J13" s="2"/>
+      <c r="N13">
+        <v>20</v>
+      </c>
       <c r="O13" s="2">
         <v>0.5625</v>
       </c>
       <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>45594</v>
       </c>
@@ -960,12 +1042,18 @@
         <v>0.41041666666666665</v>
       </c>
       <c r="J14" s="2"/>
+      <c r="N14">
+        <v>20</v>
+      </c>
       <c r="O14" s="2">
         <v>0.56597222222222221</v>
       </c>
       <c r="P14" s="2"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>45595</v>
       </c>
@@ -991,12 +1079,18 @@
         <v>19</v>
       </c>
       <c r="J15" s="2"/>
+      <c r="N15">
+        <v>20</v>
+      </c>
       <c r="O15" s="2">
         <v>0.58333333333333337</v>
       </c>
       <c r="P15" s="2"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>45596</v>
       </c>
@@ -1019,12 +1113,18 @@
         <v>0.39305555555555555</v>
       </c>
       <c r="J16" s="2"/>
+      <c r="N16">
+        <v>20</v>
+      </c>
       <c r="O16" s="2">
         <v>0.56041666666666667</v>
       </c>
       <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="U16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>45597</v>
       </c>
@@ -1047,12 +1147,18 @@
         <v>0.38333333333333336</v>
       </c>
       <c r="J17" s="2"/>
+      <c r="N17">
+        <v>15</v>
+      </c>
       <c r="O17" s="2">
         <v>0.56944444444444442</v>
       </c>
       <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="U17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>45598</v>
       </c>
@@ -1075,12 +1181,18 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="J18" s="2"/>
+      <c r="N18">
+        <v>15</v>
+      </c>
       <c r="O18" s="2">
         <v>0.61111111111111116</v>
       </c>
       <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="U18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>45599</v>
       </c>
@@ -1120,69 +1232,188 @@
       <c r="O19" s="2">
         <v>0.59444444444444444</v>
       </c>
-      <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P19" s="2">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="Q19">
+        <v>141</v>
+      </c>
+      <c r="R19">
+        <v>77</v>
+      </c>
+      <c r="S19">
+        <v>69</v>
+      </c>
+      <c r="U19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>45600</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.39513888888888887</v>
+      </c>
+      <c r="D20">
+        <v>132</v>
+      </c>
+      <c r="E20">
+        <v>62</v>
+      </c>
+      <c r="F20">
+        <v>64</v>
+      </c>
+      <c r="G20">
+        <v>15</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="K20">
+        <v>114</v>
+      </c>
+      <c r="L20" s="3">
+        <v>70</v>
+      </c>
+      <c r="M20">
+        <v>65</v>
+      </c>
+      <c r="N20">
+        <v>15</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0.5756944444444444</v>
+      </c>
+      <c r="P20" s="2">
+        <v>0.67777777777777781</v>
+      </c>
+      <c r="Q20">
+        <v>120</v>
+      </c>
+      <c r="R20">
+        <v>73</v>
+      </c>
+      <c r="S20">
+        <v>60</v>
+      </c>
+      <c r="U20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>45601</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C21" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D21">
+        <v>116</v>
+      </c>
+      <c r="E21">
+        <v>71</v>
+      </c>
+      <c r="F21">
+        <v>61</v>
+      </c>
+      <c r="G21">
+        <v>15</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.37638888888888888</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.55347222222222225</v>
+      </c>
+      <c r="K21">
+        <v>105</v>
+      </c>
+      <c r="L21" s="3">
+        <v>69</v>
+      </c>
+      <c r="M21">
+        <v>74</v>
+      </c>
+      <c r="N21">
+        <v>15</v>
+      </c>
+      <c r="O21" s="2">
+        <v>0.5541666666666667</v>
+      </c>
+      <c r="P21" s="2">
+        <v>0.68194444444444446</v>
+      </c>
+      <c r="Q21">
+        <v>114</v>
+      </c>
+      <c r="R21">
+        <v>71</v>
+      </c>
+      <c r="S21">
+        <v>64</v>
+      </c>
+      <c r="U21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>45602</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>45603</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>45604</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>45605</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>45606</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>45607</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>45608</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>45609</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>45610</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>45611</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>45612</v>
       </c>

</xml_diff>